<commit_message>
till Bottom halves & deffering works
</commit_message>
<xml_diff>
--- a/improvement/quick_notes.xlsx
+++ b/improvement/quick_notes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="interview preparation" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="441">
   <si>
     <t>Sr No</t>
   </si>
@@ -1318,7 +1318,8 @@
     <t>process descriptor</t>
   </si>
   <si>
-    <t>struct task_struct
+    <t>
+Struct task_struct
     - pid
     - state
     - stack
@@ -1329,7 +1330,8 @@
     - parent, child &amp; sibling pd info
     - resources information:: open files, devices
     - singal related information
-    - etc.</t>
+    - etc.
+</t>
   </si>
   <si>
     <t>process descriptor allocation</t>
@@ -1356,17 +1358,22 @@
     <t>PID</t>
   </si>
   <si>
-    <t>- The system identifies processes by a unique process identification value or PID.
-- may increase the maximum value via /proc/sys/kernel/pid_max .</t>
-  </si>
-  <si>
-    <t>current_thread_info()-&gt;task; return pointer to current executing pd</t>
+    <t>
+- The system identifies processes by a unique process identification value or PID.
+- may increase the maximum value via /proc/sys/kernel/pid_max .
+</t>
+  </si>
+  <si>
+    <t>
+Current_thread_info()-&gt;task; return pointer to current executing pd
+</t>
   </si>
   <si>
     <t>state</t>
   </si>
   <si>
-    <t>Process State
+    <t>
+Process State
 - TASK_READY:: Existing task calls fork() and creates a new process.ready but not running.
 - TASK_RUNNING:: running.
 - TASK_TERMINATE:: Task exits via do_exit.
@@ -1377,22 +1384,27 @@
     <t>manupulating current process state</t>
   </si>
   <si>
-    <t>- set_task_state(task, state); or task-&gt;state = state;
-- The method set_current_state(state) is synonymous to set_task_state(current,state) . See &lt;linux/sched.h&gt; for the implementation of these and related functions.</t>
+    <t>
+- set_task_state(task, state); or task-&gt;state = state;
+- The method set_current_state(state) is synonymous to set_task_state(current,state) . See &lt;linux/sched.h&gt; for the implementation of these and related functions.
+</t>
   </si>
   <si>
     <t>Process Context</t>
   </si>
   <si>
-    <t>- Normal program execution occurs in user-space.When a program executes a system call or triggers an exception, it enters kernel-space.
+    <t>
+- Normal program execution occurs in user-space.When a program executes a system call or triggers an exception, it enters kernel-space.
 - At this point, the kernel is said to be “executing on behalf of the process” and is in process context.When in process context, the current macro is valid. 
-- Upon exiting the kernel, the process resumes execution in user-space, unless a higher-priority process has become runnable in the interim, in which case the scheduler is invoked to select the higher priority process.</t>
+- Upon exiting the kernel, the process resumes execution in user-space, unless a higher-priority process has become runnable in the interim, in which case the scheduler is invoked to select the higher priority process.
+</t>
   </si>
   <si>
     <t>process tree</t>
   </si>
   <si>
-    <t>- Each task_struct has a pointer to the parent’s task_struct , named parent , and a list of children, named children.
+    <t>
+- Each task_struct has a pointer to the parent’s task_struct , named parent , and a list of children, named children.
 - from the current proccess descriptor, it is possible to obtain the process descriptor of its parent.
     struct task_struct *my_parent = current-&gt;parent;
 - it is possible to iterate over a process’s children with
@@ -1410,19 +1422,22 @@
     for_each_process(task) {
     /* this pointlessly prints the name and PID of each task */
     printk(“%s[%d]\n”, task-&gt;comm, task-&gt;pid);
-    }</t>
+    }
+</t>
   </si>
   <si>
     <t>Kernel Threads</t>
   </si>
   <si>
-    <t>- The significant difference between kernel threads and normal processes is that kernel threads do not have an address space. (Their mm pointer, which points at their address space, is NULL .) 
+    <t>
+- The significant difference between kernel threads and normal processes is that kernel threads do not have an address space. (Their mm pointer, which points at their address space, is NULL .) 
 - They operate only in kernel-space and do not context switch into user-space. Kernel threads, however, are schedulable and preemptable, the same as normal processes.
 - a kernel thread can be created only by another kernel thread.
 - The interface, declared in &lt;linux/kthread.h&gt; , for spawning a new kernel thread from an existing one is kthread_create()::
 - The process is created in an unrunnable state; it will not start running until explicitly woken up via wake_up_process() .A process can be created and made runnable with a single function, kthread_run() :
 - This routine, implemented as a macro, simply calls both kthread_create() and wake_up_process() :
-- a kernel thread continues to exist until it calls do_exit() or another part of the kernel calls kthread_stop() , passing in the address of the task_struct structure returned by kthread_create() :</t>
+- a kernel thread continues to exist until it calls do_exit() or another part of the kernel calls kthread_stop() , passing in the address of the task_struct structure returned by kthread_create() :
+</t>
   </si>
   <si>
     <t>$ps -ef
@@ -1447,17 +1462,21 @@
     <t>The Dilemma of the Parentless Task</t>
   </si>
   <si>
-    <t>- The solution is to reparent a task’s children on exit to either another process in the current thread group or, if that fails, the init process.
+    <t>
+- The solution is to reparent a task’s children on exit to either another process in the current thread group or, if that fails, the init process.
 - above is done using api::
-    static struct task_struct *find_new_reaper(struct task_struct *father)</t>
+    static struct task_struct *find_new_reaper(struct task_struct *father)
+</t>
   </si>
   <si>
     <t>Process Scheduler</t>
   </si>
   <si>
-    <t>- The process scheduler decides which process runs, when, and for how long
+    <t>
+- The process scheduler decides which process runs, when, and for how long
 - The idea behind the scheduler is simple.To best utilize processor time, assuming there are more runnable processes than processors in a system.
-- These processes are waiting to run. Deciding which process runs next, given a set of runnable processes, is the fundamental decision that the scheduler must make.</t>
+- These processes are waiting to run. Deciding which process runs next, given a set of runnable processes, is the fundamental decision that the scheduler must make.
+</t>
   </si>
   <si>
     <t>policy</t>
@@ -1472,17 +1491,21 @@
     <t>Process Priority</t>
   </si>
   <si>
-    <t>- A common type of scheduling algorithm is priority-based scheduling.
+    <t>
+- A common type of scheduling algorithm is priority-based scheduling.
 - processes with the same priority are scheduled round-robin (one after the next, repeating).
 - The Linux kernel implements two separate priority ranges.
     - The first is the nice value, a number from –20 to +19 with a default of 0. Larger nice values correspond to a lower priority. eg $ps -el
-    - The second range is the real-time priority.The values are configurable, but by default range from 0 to 99, inclusive. Opposite from nice values, higher real-time priority values correspond to a greater priority. eg $ ps -eo state,uid,pid,ppid,rtprio,time,comm</t>
+    - The second range is the real-time priority.The values are configurable, but by default range from 0 to 99, inclusive. Opposite from nice values, higher real-time priority values correspond to a greater priority. eg $ ps -eo state,uid,pid,ppid,rtprio,time,comm
+</t>
   </si>
   <si>
     <t>Timeslice</t>
   </si>
   <si>
-    <t>- The timeslice is the numeric value that represents how long a task can run until it is pre-empted.</t>
+    <t>
+- The timeslice is the numeric value that represents how long a task can run until it is pre-empted.
+</t>
   </si>
   <si>
     <t>System calls</t>
@@ -1491,7 +1514,8 @@
     <t>System Call Implementation</t>
   </si>
   <si>
-    <t>- Implementing System Calls
+    <t>
+- Implementing System Calls
     - kernel/sys.c
         #include &lt;asm/page.h&gt;
         /*
@@ -1511,14 +1535,17 @@
     .long sys_foo
 - For each supported architecture, define the syscall number in &lt;asm/unistd.h&gt;.
     #define __NR_foo 338
-- Compile the syscall into the kernel image (as opposed to compiling as a module).</t>
+- Compile the syscall into the kernel image (as opposed to compiling as a module).
+</t>
   </si>
   <si>
     <t>System Call Context</t>
   </si>
   <si>
-    <t>- In process context, the kernel is capable of sleeping (for example, if the system call blocks on a call or explicitly calls schedule()) and is fully preemptible.
-- preemptible implies that, like user-space, the current task may be preempted by another task. Because the new task may then execute the same system call, care must be exercised to ensure that system calls are reentrant.</t>
+    <t>
+- In process context, the kernel is capable of sleeping (for example, if the system call blocks on a call or explicitly calls schedule()) and is fully preemptible.
+- preemptible implies that, like user-space, the current task may be preempted by another task. Because the new task may then execute the same system call, care must be exercised to ensure that system calls are reentrant.
+</t>
   </si>
   <si>
     <t>Accessing the System Call from User-Space</t>
@@ -1549,7 +1576,8 @@
     <t>The Linked List Structure</t>
   </si>
   <si>
-    <t>- The kernel provides a family of routines to manipulate linked lists.
+    <t>
+- The kernel provides a family of routines to manipulate linked lists.
     - the list_add() method adds a new node to an existing linked list.These methods, however, are generic:They accept only list_head structures.
     - Using the macro container_of() , we can easily find the parent structure containing any given member variable.
 </t>
@@ -1566,7 +1594,8 @@
     <t>Defining a Linked List</t>
   </si>
   <si>
-    <t>- As shown, a list_head by itself is worthless; it is normally embedded inside your own structure:
+    <t>
+- As shown, a list_head by itself is worthless; it is normally embedded inside your own structure:
 struct fox {
     unsigned long tail_length; /*length in centimeters of tail */ 
     unsigned long weight;      /*weight in kilograms */ 
@@ -1579,13 +1608,16 @@
 red_fox-&gt;tail_length = 40;
 red_fox-&gt;weight = 6;
 red_fox-&gt;is_fantastic = false;
-INIT_LIST_HEAD(&amp;red_fox-&gt;list);</t>
+INIT_LIST_HEAD(&amp;red_fox-&gt;list);
+</t>
   </si>
   <si>
     <t>List Heads</t>
   </si>
   <si>
-    <t>This defines and initializes a list_head named fox_list .</t>
+    <t>
+This defines and initializes a list_head named fox_list .
+</t>
   </si>
   <si>
     <t>static LIST_HEAD(fox_list);</t>
@@ -1594,26 +1626,31 @@
     <t>Manipulating Linked Lists</t>
   </si>
   <si>
-    <t>The functions are implemented as inline functions in generic C and can be found in &lt;linux/list.h&gt; .</t>
+    <t>
+The functions are implemented as inline functions in generic C and can be found in &lt;linux/list.h&gt; .
+</t>
   </si>
   <si>
     <t>Adding a Node to a Linked List</t>
   </si>
   <si>
-    <t>- To add a node to a linked list:
+    <t>
+- To add a node to a linked list:
     list_add(struct list_head *new, struct list_head *head)
     This function adds the new node to the given list immediately after the head node. Because the list is circular and generally has no concept of first or last nodes, you can pass any element for head .
 - assume we had a new struct fox that we wanted to add to the fox_list list.We’d do this:
     list_add(&amp;f-&gt;list, &amp;fox_list);
     To add a node to the end of a linked list:
     list_add_tail(struct list_head *new, struct list_head *head)
-    This function adds the new node to the given list immediately before the head node.As with list_add()</t>
+    This function adds the new node to the given list immediately before the head node.As with list_add()
+</t>
   </si>
   <si>
     <t>Deleting a Node from a Linked List</t>
   </si>
   <si>
-    <t>- list_del(struct list_head *entry)
+    <t>
+- list_del(struct list_head *entry)
     This function removes the element entry from the list. Note that it does not free any memory belonging to entry or the data structure in which it is embedded; this function merely removes the element from the list.After calling this, you would typically destroy your data structure and the list_head inside it.
     list_del(&amp;f-&gt;list);
     Note the function does not receive as input fox_list.
@@ -1632,7 +1669,8 @@
     <t>Traversing Linked Lists</t>
   </si>
   <si>
-    <t>    - The Basic Approach
+    <t>
+    - The Basic Approach
         The first is a pointer used to point to the current entry; it is a temporary variable that you must provide.The second is the list_head acting as the head node of the list you want to traverse (see the earlier section, “List Heads”). On each iteration of the loop, the first parameter points to the next entry in the list, until each entry has been visited.
             struct list_head *p;
             struct fox *f;
@@ -1655,30 +1693,37 @@
     <t>Iterating Through a List Backward</t>
   </si>
   <si>
-    <t>list_for_each_entry_reverse(pos, head, member)</t>
+    <t>
+List_for_each_entry_reverse(pos, head, member)
+</t>
   </si>
   <si>
     <t>Iterating While Removing</t>
   </si>
   <si>
-    <t>The standard methods rely on the fact that the list entries are not changing out from under them, and thus if the current entry is removed in the body of the loop, the subsequent iteration cannot advance to the next (or previous) pointer.
-    list_for_each_entry_safe(pos, next, head, member)</t>
+    <t>
+The standard methods rely on the fact that the list entries are not changing out from under them, and thus if the current entry is removed in the body of the loop, the subsequent iteration cannot advance to the next (or previous) pointer.
+    list_for_each_entry_safe(pos, next, head, member)
+</t>
   </si>
   <si>
     <t>kfifo</t>
   </si>
   <si>
-    <t>The kfifo object maintains two off- sets into the queue: 
+    <t>
+The kfifo object maintains two off- sets into the queue: 
     - an in offset and an out offset.The in offset is the location in the queue to which the next enqueue will occur.
     - The out offset is the location in the queue from which the next dequeue will occur.
     - When the out offset is equal to the in offset, the queue is empty.
-    - When the in offset is equal to the length of the queue, no more data can be enqueued until the queue is reset.</t>
+    - When the in offset is equal to the length of the queue, no more data can be enqueued until the queue is reset.
+</t>
   </si>
   <si>
     <t>Creating Queue</t>
   </si>
   <si>
-    <t>- below function creates and initializes a kfifo with a queue of size bytes.The kernel uses the gfp mask gfp_mask to allocate the queue.
+    <t>
+- below function creates and initializes a kfifo with a queue of size bytes.The kernel uses the gfp mask gfp_mask to allocate the queue.
 - Upon success, kfifo_alloc() returns zero; on error it returns a negative error code.
 struct kfifo fifo;
 int ret;
@@ -1692,13 +1737,15 @@
 Statically declaring a kfifo is simpler, but less common:
 DECLARE_KFIFO(name, size);
 INIT_KFIFO(name);
-This creates a static kfifo named name with a queue of size bytes.As before, sizemust be a power of 2.</t>
+This creates a static kfifo named name with a queue of size bytes.As before, sizemust be a power of 2.
+</t>
   </si>
   <si>
     <t>Enqueuing Data</t>
   </si>
   <si>
-    <t>- When your kfifo is created and initialized, enqueuing data into the queue is performed via the kfifo_in() function:
+    <t>
+- When your kfifo is created and initialized, enqueuing data into the queue is performed via the kfifo_in() function:
 - This function copies the len bytes starting at from into the queue represented by fifo . 
 - On success it returns the number of bytes enqueued. If less than len bytes are free in the queue, the function copies only up to the amount of available bytes.Thus the return value can be less than len or even zero, if nothing was copied.
 </t>
@@ -1710,17 +1757,20 @@
     <t>Dequeue data</t>
   </si>
   <si>
-    <t>- This function copies at most len bytes from the queue pointed at by fifo to the buffer pointed at by to . On success the function returns the number of bytes copied. If less than len bytes are in the queue, the function copies less than requested.
+    <t>
+- This function copies at most len bytes from the queue pointed at by fifo to the buffer pointed at by to . On success the function returns the number of bytes copied. If less than len bytes are in the queue, the function copies less than requested.
     unsigned int kfifo_out(struct kfifo *fifo, void *to, unsigned int len);
 - When dequeued, data is no longer accessible from the queue.This is the normal usage of a queue, but if you want to “peek” at data within the queue without removing it, you can use kfifo_out_peek() :
     unsigned int kfifo_out_peek(struct kfifo *fifo, void *to, unsigned int len, unsigned offset);
-    This works the same as kfifo_out() , except that the out offset is not incremented,The parameter offset specifies an index into the queue; specify zero to read from the head of the queue, as kfifo_out() does.</t>
+    This works the same as kfifo_out() , except that the out offset is not incremented,The parameter offset specifies an index into the queue; specify zero to read from the head of the queue, as kfifo_out() does.
+</t>
   </si>
   <si>
     <t>Obtaining the Size of a Queue</t>
   </si>
   <si>
-    <t>- To obtain the total size in bytes of the buffer used to store a kfifo’s queue, call kfifo_size() :
+    <t>
+- To obtain the total size in bytes of the buffer used to store a kfifo’s queue, call kfifo_size() :
 - kfifo_len() to obtain the number of bytes enqueued in a kfifo:
 - number of bytes available to write into a kfifo, call kfifo_avail() :
 - kfifo_is_empty() and kfifo_is_full() return nonzero if the given kfifo is empty or full, respectively, and zero if not:
@@ -1737,7 +1787,8 @@
     <t>Resetting and Destroying the Queue</t>
   </si>
   <si>
-    <t>- To reset a kfifo, jettisoning all the contents of the queue, call kfifo_reset() :
+    <t>
+- To reset a kfifo, jettisoning all the contents of the queue, call kfifo_reset() :
 - To destroy a kfifo allocated with kfifo_alloc() , call kfifo_free() :
 - If you created your kfifo with kfifo_init() , it is your responsibility to free the associated buffer.
 </t>
@@ -1745,6 +1796,410 @@
   <si>
     <t>static inline void kfifo_reset(struct kfifo *fifo);
 void kfifo_free(struct kfifo *fifo);
+</t>
+  </si>
+  <si>
+    <t>Top Halves Versus Bottom Halves</t>
+  </si>
+  <si>
+    <t>
+- The top half is run immediately upon receipt of the interrupt and performs only the work that is time-critical, such as acknowledging receipt of the interrupt or resetting the hardware.
+- Work that can be performed later is deferred until the bottom half.The bottom half runs in the future, at a more convenient time, with all interrupts enabled.
+    Let’s look at an example of the top-half/bottom-half dichotomy, using the network card.
+    - The interrupt runs, acknowledges the hardware, copies the new networking packets into main memory, and readies the network card for more packets.These jobs are the important, time-critical, and hardware-specific work.
+    - The rest of the processing and handling of the packets occurs later, in the bottom half.
+</t>
+  </si>
+  <si>
+    <t>Interrupts and Interrupt Handlers</t>
+  </si>
+  <si>
+    <t>Registering an Interrupt Handler</t>
+  </si>
+  <si>
+    <t>
+- Drivers can register an interrupt handler and enable a given interrupt line for handling with the function request_irq() , which is declared in &lt;linux/interrupt.h&gt; :
+/* request_irq: allocate a given interrupt line */
+int request_irq (unsigned int irq, irq_handler_t handler, const char *name, void *dev)
+    - The first parameter, irq , specifies the interrupt number to allocate. For some devices, such as the system timer or keyboard, this value is typically hard-coded. For most other devices, it is probed or otherwise determined programmatically and dynamically.
+    - The second parameter, handler , is a function pointer to the actual interrupt handler that services this interrupt.This function is invoked whenever the operating system
+receives the interrupt.
+    typedef irqreturn_t (*irq_handler_t)(int, void *);
+    - The third parameter, flags , can be either zero or a bit mask of one or more of the flags defined in &lt;linux/interrupt.h&gt; .Among these flags, the most important are
+    IRQF_DISABLED:: When set, this flag instructs the kernel to disable all interrupts when executing this interrupt handler.When unset, interrupt handlers run with all interrupts except their own enabled.
+    IRQF_SAMPLE_RANDOM:: This flag specifies that interrupts generated by this device should contribute to the kernel entropy pool
+    IRQF_TIMER:: This flag specifies that this handler processes interrupts for the system timer.
+    IRQF_SHARED:: This flag specifies that the interrupt line can be shared among multiple interrupt handlers. Each handler registered on a given line must specify this
+flag; otherwise, only one handler can exist per line.
+    - The fourth parameter, name , is an ASCII text representation of the device associated with the interrupt. These text names are used by /proc/irq and /proc/interrupts for communication with the user.
+    - The fifth parameter, dev , is used for shared interrupt lines. Without this parameter, it would be impossible for the kernel to know which handler to remove on a given interrupt line.You can pass NULL here if the line is not shared, but you must pass a unique cookie if your interrupt line is shared.
+    - On success, request_irq() returns zero.A nonzero value indicates an error, in which case the specified interrupt handler was not registered.
+- Note that request_irq() can sleep and therefore cannot be called from interrupt context or other situations where code cannot block.
+- On registration, an entry corresponding to the interrupt is created in /proc/irq .
+</t>
+  </si>
+  <si>
+    <t>Freeing an Interrupt Handler</t>
+  </si>
+  <si>
+    <t>
+- When your driver unloads, you need to unregister your interrupt handler and potentially disable the interrupt line.To do this, call
+    void free_irq(unsigned int irq, void *dev)
+- If the specified interrupt line is not shared, this function removes the handler and disables the line. If the interrupt line is shared, the handler identified via dev is removed, but the interrupt line is disabled only when the last handler is removed.
+</t>
+  </si>
+  <si>
+    <t>Writing an Interrupt Handler</t>
+  </si>
+  <si>
+    <t>
+- The following is a declaration of an interrupt handler:
+    static irqreturn_t intr_handler(int irq, void *dev)
+    - The first parameter, irq , is the numeric value of the interrupt line the handler is servicing.
+    - The second parameter, dev , is a generic pointer to the same dev that was given to request_irq() when the interrupt handler was registered. If this value is unique (which
+is required to support sharing), it can act as a cookie to differentiate between multiple devices potentially using the same interrupt handler.
+    - The return value of an interrupt handler is the special type irqreturn_t .An interrupt handler can return two special values, IRQ_NONE or IRQ_HANDLED. f the interrupt handler was correctly invoked, and its device did indeed cause the interrupt.Alternatively, IRQ_RETVAL(val) may be used. If val is nonzero, this macro returns IRQ_HANDLED. Otherwise, the macro returns IRQ_NONE .
+</t>
+  </si>
+  <si>
+    <t>Interrupt Context</t>
+  </si>
+  <si>
+    <t>
+- When executing an interrupt handler, the kernel is in interrupt context.
+- Interrupt context, on the other hand, is not associated with a process.The current macro is not relevant (although it points to the interrupted process).Without a backing process, interrupt context cannot sleep.
+- Interrupt context is time-critical because the interrupt handler interrupts other code.
+- Interrupt handlers were given their own stack, one stack per processor, one page in size.This stack is referred to as the interrupt stack.
+- Your interrupt handler should not care what stack setup is in use or what the size of the kernel stack is.Always use an absolute minimum amount of stack space.
+</t>
+  </si>
+  <si>
+    <t>Interrupt Control</t>
+  </si>
+  <si>
+    <t>
+- Disabling and Enabling Interrupts
+    local_irq_disable() Disables local interrupt delivery
+    local_irq_enable() Enables local interrupt delivery
+    local_irq_save() Saves the current state of local interrupt delivery and then disables it
+    local_irq_restore() Restores local interrupt delivery to the given state
+- Disabling a Specific Interrupt Line
+    disable_irq() Disables the given interrupt line and ensures no handler on the line is executing before returning
+    disable_irq_nosync() Disables the given interrupt line
+    enable_irq() Enables the given interrupt line
+    irqs_disabled() Returns nonzero if local interrupt delivery is disabled; otherwise returns zero
+    synchronize_irq(unsigned int irq); waits for a specific interrupt handler to exit, if it is executing, before returning.
+- Status of the Interrupt System
+    in_interrupt() Returns nonzero if in interrupt context and zero if in process context
+    in_irq() Returns nonzero if currently executing an interrupt handler and zero otherwise
+</t>
+  </si>
+  <si>
+    <t>Bottom Halves and Deferring Work</t>
+  </si>
+  <si>
+    <t>Task Queues</t>
+  </si>
+  <si>
+    <t>
+It also was not lightweight enough for performancecritical subsystems, such as networking.
+</t>
+  </si>
+  <si>
+    <t>Softirqs and Tasklets</t>
+  </si>
+  <si>
+    <t>
+- Softirqs 
+    - Softirqs are a set of statically defined bottom halves that can run simultaneously on any processor; even two of the same type can run concurrently.
+    - Softirqs are useful when performance is critical, such as with networking.
+    - softirqs must be registered statically at compile time.
+- Tasklets
+    - Tasklets are flexible, dynamically created bottom halves built on top of softirqs.
+    - Two different tasklets can run concurrently on different processors, but two of the same type of tasklet cannot run simultaneously.Thus, tasklets are a good trade-off between performance and ease of use.
+</t>
+  </si>
+  <si>
+    <t>Softirqs</t>
+  </si>
+  <si>
+    <t>
+- Softirqs are rarely used directly; tasklets are a much more common form of bottom half.Nonetheless, because tasklets are built on softirqs.
+- A softirq never preempts another softirq.The only event that can preempt a softirq is an interrupt handler.Another softirq—even the same one—can run on another processor, however.
+</t>
+  </si>
+  <si>
+    <t>Implementing Softirqs</t>
+  </si>
+  <si>
+    <t>
+- Softirqs are statically allocated at compile time. Unlike tasklets, you cannot dynamically register and destroy softirqs. 
+- Softirqs are represented by the softirq_action structure, which is defined in &lt;linux/interrupt.h&gt; :
+    struct softirq_action {void (*action)(struct softirq_action *);};
+- A 32-entry array of this structure is declared in kernel/softirq.c :
+    static struct softirq_action softirq_vec[NR_SOFTIRQS];
+    The kernel enforces a limit of 32 registered softirqs; in the current kernel, however, only nine exist
+- Softirq Handler:: 
+    The prototype of a softirq handler, action , looks like
+    void softirq_handler(struct softirq_action *)
+- Executing Softirqs
+    - A registered softirq must be marked before it will execute.This is called raising the softirq.
+    - Usually, an interrupt handler marks its softirq for execution before returning.
+</t>
+  </si>
+  <si>
+    <t>Assigning an Index</t>
+  </si>
+  <si>
+    <t>
+    Tasklet Priority Softirq Description
+    HI_SOFTIRQ 0 High-priority tasklets
+    TIMER_SOFTIRQ 1 Timers
+    NET_TX_SOFTIRQ 2 Send network packets
+    NET_RX_SOFTIRQ 3 Receive network packets
+    BLOCK_SOFTIRQ 4 Block devices
+    TASKLET_SOFTIRQ 5 Normal priority tasklets
+    SCHED_SOFTIRQ 6 Scheduler
+    HRTIMER_SOFTIRQ 7 High-resolution timers
+    RCU_SOFTIRQ 8 RCU locking
+</t>
+  </si>
+  <si>
+    <t>Registering Your Handler</t>
+  </si>
+  <si>
+    <t>
+- The softirq handler is registered at run-time via open_softirq(),which takes two parameters: the softirq’s index and its handler function.
+- The networking subsystem, for example, registers its softirqs like this, in net/core/dev.c :
+    open_softirq(NET_TX_SOFTIRQ, net_tx_action);
+    open_softirq(NET_RX_SOFTIRQ, net_rx_action);
+- The softirq handlers run with interrupts enabled and cannot sleep.While a handler runs, softirqs on the current processor are disabled.
+- Another processor, however, can execute other softirqs. If the same softirq is raised again while it is executing, another processor can run it simultaneously.
+- This means that any shared data—even global data used only within the softirq handler—needs proper locking.
+- This is an important point, and it is the reason tasklets are usually preferred.
+</t>
+  </si>
+  <si>
+    <t>Raising Your Softirq</t>
+  </si>
+  <si>
+    <t>
+- To mark it pending, so it is run at the next invocation of do_softirq() , call raise_softirq() . 
+- For example, the networking subsystem would call,
+    raise_softirq(NET_TX_SOFTIRQ);
+- This raises the NET_TX_SOFTIRQ softirq. Its handler, net_tx_action() , runs the next time the kernel executes softirqs.
+- This function disables interrupts prior to actually raising the softirq and then restores them to their previous state. 
+- If interrupts are already off, the function raise_softirq_irqoff() can be used as a small optimization. For example
+    /*
+    * interrupts must already be off!
+    */
+    raise_softirq_irqoff(NET_TX_SOFTIRQ);
+</t>
+  </si>
+  <si>
+    <t>Tasklets</t>
+  </si>
+  <si>
+    <t>
+Tasklets are a bottom-half mechanism built on top of softirqs.As mentioned, they have nothing to do with tasks.
+</t>
+  </si>
+  <si>
+    <t>Implementing tasklets</t>
+  </si>
+  <si>
+    <t>
+- tasklets are represented by two softirqs: HI_SOFTIRQ and TASKLET_SOFTIRQ .
+- The only difference in these types is that the HI_SOFTIRQ -based tasklets run prior to the TASKLET_SOFTIRQ based tasklets.
+- The Tasklet Structure
+    - Tasklets are represented by the tasklet_struct structure. Each structure represents a unique tasklet.The structure is declared in &lt;linux/interrupt.h&gt; :
+        struct tasklet_struct {
+            struct tasklet_struct *next;
+            unsigned long state;
+            atomic_t count;
+            void (*func)(unsigned long);
+            unsigned long data;
+        };
+        - The func member is the tasklet handler (the equivalent of action to a softirq) and receives data as its sole argument.
+        - The state member is exactly zero, TASKLET_STATE_SCHED , or TASKLET_STATE_RUN .
+        - The count field is used as a reference count for the tasklet. If it is nonzero, the tasklet is disabled and cannot run; if it is zero, the tasklet is enabled and can run if marked pending
+- Scheduling Tasklets
+    - Tasklets are scheduled via the tasklet_schedule() and tasklet_hi_schedule() functions, which receive a pointer to the tasklet’s tasklet_struct as their lone argument.
+    - Each function ensures that the provided tasklet is not yet scheduled and then calls __tasklet_schedule() and __tasklet_hi_schedule() as appropriate.
+    - The two functions are similar. (The difference is that one uses TASKLET_SOFTIRQ and one uses HI_SOFTIRQ. )
+    - the steps tasklet_schedule() undertakes:
+        1. Check whether the tasklet’s state is TASKLET _ STATE_SCHED . If it is, the tasklet is already scheduled to run and the function can immediately return.
+        2. Call __tasklet_schedule() .
+        3. Save the state of the interrupt system, and then disable local interrupts.This ensures that nothing on this processor will mess with the tasklet code while tasklet_schedule() is manipulating the tasklets.
+        4. Add the tasklet to be scheduled to the head of the tasklet_vec or tasklet_hi_vec linked list, which is unique to each processor in the system.
+        5. Raise the TASKLET_SOFTIRQ or HI_SOFTIRQ softirq, so do_softirq() executes this tasklet in the near future.
+        6. Restore interrupts to their previous state and return.
+</t>
+  </si>
+  <si>
+    <t>Using Tasklets</t>
+  </si>
+  <si>
+    <t>
+- Declaring Your Tasklet
+    - statically create the tasklet, use one of two macros in &lt;linux/interrupt.h&gt; :
+        DECLARE_TASKLET(name, func, data)
+        DECLARE_TASKLET_DISABLED(name, func, data);
+        - When the tasklet is scheduled, the given function func is executed and passed the argument data.
+        - The first macro creates the tasklet with a count of zero, and the tasklet is enabled.
+        - The second macro sets count to one, and the tasklet is disabled
+    - To initialize a tasklet given an indirect reference (a pointer) to a dynamically created struct tasklet_struct , t , call tasklet_init() :
+        tasklet_init(t, tasklet_handler, dev); /* dynamically as opposed to statically */
+- Writing Your Tasklet Handler
+    - The tasklet handler must match the correct prototype:
+        void tasklet_handler(unsigned long data)
+    - As with softirqs, tasklets cannot sleep.This means you cannot use semaphores or other blocking functions in a tasklet.
+    - Tasklets also run with all interrupts enabled, so you must take precautions (for example, disable interrupts and obtain a lock) if your tasklet shares data with an interrupt handler. 
+    - If your tasklet shares data with another tasklet or softirq, you need to use proper locking.
+- Scheduling Your Tasklet
+    - To schedule a tasklet for execution, tasklet_schedule() is called and passed a pointer to the relevant tasklet_struct :
+        tasklet_schedule(&amp;my_tasklet); /* mark my_tasklet as pending */
+    - After a tasklet is scheduled, it runs once at some time in the near future. 
+    - If the same tasklet is scheduled again, before it has had a chance to run, it still runs only once. 
+    - If it is already running, for example on another processor, the tasklet is rescheduled and runs again.
+    - Also we can enable and disble takslet
+        tasklet_disable(&amp;my_tasklet);
+        /* tasklet is now disabled */
+        /* we can now do stuff knowing that the tasklet cannot run .. */
+        tasklet_enable(&amp;my_tasklet);
+        /* tasklet is now enabled */
+</t>
+  </si>
+  <si>
+    <t>Work Queues</t>
+  </si>
+  <si>
+    <t>
+- Work queues defer work into a kernel thread—this bottom half always runs in process context.
+- Thus, code deferred to a work queue has all the usual benefits of process context. 
+- Most important, work queues are schedulable and can therefore sleep.
+</t>
+  </si>
+  <si>
+    <t>Implementing Work Queues</t>
+  </si>
+  <si>
+    <t>
+- Work queues let your driver create a special worker thread to handle deferred work.
+- The work queue subsystem, however, implements and provides a default worker thread for handling work.
+- The default worker threads are called events/n where n is the processor number; there is one per processor.
+- The default worker thread handles deferred work from multiple locations. Many drivers in the kernel defer their bottom-half work to the default thread.
+- Unless a driver or subsystem has a strong requirement for creating its own thread, the default thread is preferred.
+</t>
+  </si>
+  <si>
+    <t>Data Structures Representing the Threads</t>
+  </si>
+  <si>
+    <t>
+- The worker threads are represented by the workqueue_struct structure defined in kernel/workqueue.c:
+/*
+* The externally visible workqueue abstraction is an array of
+* per-CPU workqueues:
+*/
+struct workqueue_struct {
+    struct cpu_workqueue_struct cpu_wq[NR_CPUS];
+    struct list_head list;
+    const char *name;
+    int singlethread;
+    int freezeable;
+    int rt;
+};  
+- cpu_workqueue_struct, one per possible processor on the system. Because the worker threads exist on each processor in the system, there is one of these structures per worker thread, per processor, on a given machine.
+struct cpu_workqueue_struct {
+    spinlock_t lock; /* lock protecting this structure */
+    struct list_head worklist; /* list of work */
+    wait_queue_head_t more_work;
+    struct work_struct *current_struct;
+    struct workqueue_struct *wq; /* associated workqueue_struct */
+    task_t *thread; /* associated thread */
+};
+- Note that each type of worker thread has one workqueue_struct associated to it. Inside, there is one cpu_workqueue_struct for every thread and, thus, every processor, because there is one worker thread on each processor.
+</t>
+  </si>
+  <si>
+    <t>Data Structures Representing the Work</t>
+  </si>
+  <si>
+    <t>
+- The work is represented by the work_struct structure, defined in &lt;linux/workqueue.h&gt; :
+    struct work_struct {
+        atomic_long_t data;
+        struct list_head entry;
+        work_func_t func;
+    };
+</t>
+  </si>
+  <si>
+    <t>Using Work Queues</t>
+  </si>
+  <si>
+    <t>
+We cover the default events queue first and then look at creating new worker threads.
+- Creating Work
+    - The first step is actually creating some work to defer.To create the structure statically at runtime, use DECLARE_WORK :
+        DECLARE_WORK(name, void (*func)(void *), void *data);
+        - This statically creates a work_struct structure named name with handler function func and argument data . Alternatively, you can create work at runtime via a pointer:
+        INIT_WORK(struct work_struct *work, void (*func)(void *), void *data);
+        - This dynamically initializes the work queue pointed to by work with handler function
+- Work Queue Handler
+    - The prototype for the work queue handler is 
+        void work_handler(void *data)
+    - A worker thread executes this function, and thus, the function runs in process context. By default, interrupts are enabled and no locks are held.
+    - the work handlers cannot access user-space memory because there is no associated user-space memory map for kernel threads.
+    - The kernel can access user memory only when running on behalf of a user-space process, such as when executing a system call. Only then is user memory mapped in.
+- Scheduling Work
+    - To queue a given work’s handler function with the default events worker threads, simply call 
+        schedule_work(&amp;work);
+    - The work is scheduled immediately and is run as soon as the events worker thread on the current processor wakes up.
+    - you can schedule work to execute at a given time in the future:
+        schedule_delayed_work(&amp;work, delay);
+    - To cancel delayed work, call
+        int cancel_delayed_work(struct work_struct *work);
+- Flushing Work
+    - there is a function to flush a given work queue:
+        void flush_scheduled_work(void);
+    - This function waits until all entries in the queue are executed before returning.
+    - While waiting for any pending work to execute, the function sleeps.Therefore, you can call it only from process context.
+    - Note that this function does not cancel any delayed work.That is, any work that was scheduled via schedule_delayed_work() , and whose delay is not yet up, is not flushed
+via flush_scheduled_work(), To cancel delayed work, call
+        int cancel_delayed_work(struct work_struct *work);</t>
+  </si>
+  <si>
+    <t>Creating New Work Queues</t>
+  </si>
+  <si>
+    <t>
+- If the default queue is insufficient for your needs, you can create a new work queue and corresponding worker threads.
+- Because this creates one worker thread per processor, you should create unique work queues only if your code needs the performance of a unique set of threads.
+- You create a new work queue and the associated worker threads via a simple function:
+    struct workqueue_struct *create_workqueue(const char *name);
+    - The parameter name is used to name the kernel threads. For example, the default events queue is created via
+        struct workqueue_struct *keventd_wq;
+        keventd_wq = create_workqueue(“events”);
+        - This function creates all the worker threads (one for each processor in the system) and prepares them to handle work.
+    - Creating work is handled in the same manner regardless of the queue type. 
+    - After the work is created, the following functions are analogous to schedule_work() and schedule_delayed_work(), except that they work on the given work queue and not the default events queue.
+        int queue_work(struct workqueue_struct *wq, struct work_struct *work)
+        int queue_delayed_work(struct workqueue_struct *wq, struct work_struct *work, unsigned long delay)
+    - Finally, you can flush a wait queue via a call to the function
+        flush_workqueue(struct workqueue_struct *wq)
+</t>
+  </si>
+  <si>
+    <t>Disabling Bottom Halves</t>
+  </si>
+  <si>
+    <t>
+- Disables softirq and tasklet processing on the local processor
+    void local_bh_disable() 
+- Enables softirq and tasklet processing on the local processor
+    void local_bh_enable() 
 </t>
   </si>
 </sst>
@@ -1755,7 +2210,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1851,11 +2306,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1924,7 +2374,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2085,10 +2535,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -2168,7 +2614,7 @@
   </sheetPr>
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -2559,7 +3005,7 @@
   </sheetPr>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -2824,7 +3270,7 @@
   </sheetPr>
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>
@@ -3340,7 +3786,7 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -3409,7 +3855,7 @@
   </sheetPr>
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3979,7 +4425,7 @@
   </sheetPr>
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
@@ -4367,10 +4813,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C59" activeCellId="0" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4417,7 +4863,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="140.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="39" t="n">
         <v>2</v>
       </c>
@@ -4443,7 +4889,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="39"/>
       <c r="C7" s="38" t="s">
         <v>323</v>
@@ -4452,13 +4898,13 @@
         <v>324</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="39"/>
       <c r="D8" s="38" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="82.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="39"/>
       <c r="C9" s="38" t="s">
         <v>326</v>
@@ -4467,7 +4913,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="39"/>
       <c r="C10" s="38" t="s">
         <v>328</v>
@@ -4476,7 +4922,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="82.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="39"/>
       <c r="C11" s="38" t="s">
         <v>330</v>
@@ -4485,7 +4931,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="257" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="258.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="39"/>
       <c r="C12" s="38" t="s">
         <v>332</v>
@@ -4494,7 +4940,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="210.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="39"/>
       <c r="C13" s="38" t="s">
         <v>334</v>
@@ -4506,7 +4952,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="39"/>
       <c r="C14" s="38" t="s">
         <v>337</v>
@@ -4515,7 +4961,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="39" t="n">
         <v>3</v>
       </c>
@@ -4526,7 +4972,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="35.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="39"/>
       <c r="C16" s="38" t="s">
         <v>341</v>
@@ -4538,7 +4984,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="117.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="39"/>
       <c r="C17" s="38" t="s">
         <v>344</v>
@@ -4547,7 +4993,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="39"/>
       <c r="C18" s="38" t="s">
         <v>346</v>
@@ -4556,7 +5002,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="361.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="370.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="39" t="n">
         <v>4</v>
       </c>
@@ -4570,7 +5016,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="39"/>
       <c r="C20" s="38" t="s">
         <v>351</v>
@@ -4579,7 +5025,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="175.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="164.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="39"/>
       <c r="C21" s="38" t="s">
         <v>353</v>
@@ -4591,7 +5037,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="71.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="38" t="s">
         <v>356</v>
       </c>
@@ -4605,7 +5051,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="199" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="38" t="s">
         <v>360</v>
       </c>
@@ -4613,7 +5059,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="38" t="s">
         <v>362</v>
       </c>
@@ -4624,7 +5070,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="38" t="s">
         <v>365</v>
       </c>
@@ -4632,7 +5078,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="129.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="38" t="s">
         <v>367</v>
       </c>
@@ -4640,7 +5086,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="38" t="s">
         <v>369</v>
       </c>
@@ -4651,15 +5097,15 @@
         <v>371</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="315.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="40" t="s">
+    <row r="28" customFormat="false" ht="303.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="37" t="s">
         <v>372</v>
       </c>
       <c r="D28" s="38" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="38" t="s">
         <v>374</v>
       </c>
@@ -4667,7 +5113,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="38" t="s">
         <v>376</v>
       </c>
@@ -4675,7 +5121,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="82.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="38" t="s">
         <v>378</v>
       </c>
@@ -4683,7 +5129,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="38" t="s">
         <v>380</v>
       </c>
@@ -4691,7 +5137,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="38" t="s">
         <v>382</v>
       </c>
@@ -4702,7 +5148,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="38" t="s">
         <v>385</v>
       </c>
@@ -4710,7 +5156,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="71.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="38" t="s">
         <v>387</v>
       </c>
@@ -4721,7 +5167,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="38" t="s">
         <v>390</v>
       </c>
@@ -4730,6 +5176,196 @@
       </c>
       <c r="E36" s="38" t="s">
         <v>392</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="38" t="s">
+        <v>393</v>
+      </c>
+      <c r="D37" s="38" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="415.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="38" t="s">
+        <v>395</v>
+      </c>
+      <c r="C38" s="38" t="s">
+        <v>396</v>
+      </c>
+      <c r="D38" s="38" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="38" t="s">
+        <v>398</v>
+      </c>
+      <c r="D39" s="38" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C40" s="38" t="s">
+        <v>400</v>
+      </c>
+      <c r="D40" s="38" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="38" t="s">
+        <v>402</v>
+      </c>
+      <c r="D41" s="38" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="38" t="s">
+        <v>404</v>
+      </c>
+      <c r="D42" s="38" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="38" t="s">
+        <v>406</v>
+      </c>
+      <c r="C43" s="38" t="s">
+        <v>407</v>
+      </c>
+      <c r="D43" s="38" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="38" t="s">
+        <v>409</v>
+      </c>
+      <c r="D44" s="38" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C45" s="38" t="s">
+        <v>411</v>
+      </c>
+      <c r="D45" s="38" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="38" t="s">
+        <v>413</v>
+      </c>
+      <c r="D46" s="38" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C47" s="38" t="s">
+        <v>415</v>
+      </c>
+      <c r="D47" s="38" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C48" s="38" t="s">
+        <v>417</v>
+      </c>
+      <c r="D48" s="38" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C49" s="38" t="s">
+        <v>419</v>
+      </c>
+      <c r="D49" s="38" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C50" s="38" t="s">
+        <v>421</v>
+      </c>
+      <c r="D50" s="38" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="449.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C51" s="38" t="s">
+        <v>423</v>
+      </c>
+      <c r="D51" s="38" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="404.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C52" s="38" t="s">
+        <v>425</v>
+      </c>
+      <c r="D52" s="38" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C53" s="38" t="s">
+        <v>427</v>
+      </c>
+      <c r="D53" s="38" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C54" s="38" t="s">
+        <v>429</v>
+      </c>
+      <c r="D54" s="38" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="348.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C55" s="38" t="s">
+        <v>431</v>
+      </c>
+      <c r="D55" s="38" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C56" s="38" t="s">
+        <v>433</v>
+      </c>
+      <c r="D56" s="38" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="426.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C57" s="38" t="s">
+        <v>435</v>
+      </c>
+      <c r="D57" s="38" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C58" s="38" t="s">
+        <v>437</v>
+      </c>
+      <c r="D58" s="38" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C59" s="38" t="s">
+        <v>439</v>
+      </c>
+      <c r="D59" s="38" t="s">
+        <v>440</v>
       </c>
     </row>
   </sheetData>
@@ -4755,7 +5391,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
device and modules added
</commit_message>
<xml_diff>
--- a/improvement/quick_notes.xlsx
+++ b/improvement/quick_notes.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="633">
   <si>
     <t>Sr No</t>
   </si>
@@ -1913,8 +1913,7 @@
 </t>
   </si>
   <si>
-    <r>
-      <t>
+    <t>
 Local_irq_disable():: Disables local interrupt delivery
 local_irq_enable():: Enables local interrupt delivery
 local_irq_save():: Saves the current state of local interrupt delivery and then disables it
@@ -1926,7 +1925,6 @@
 in_interrupt():: Returns nonzero if in interrupt context and zero if in process context
 in_irq():: Returns nonzero if currently executing an interrupt handler and zero otherwise
 </t>
-    </r>
   </si>
   <si>
     <t>Bottom Halves and Deferring Work</t>
@@ -2017,8 +2015,7 @@
     <t>Raising Your Softirq</t>
   </si>
   <si>
-    <r>
-      <t>
+    <t>
 - To mark it pending, so it is run at the next invocation of do_softirq() , call raise_softirq() . 
 - For example, the networking subsystem would call,
     raise_softirq(NET_TX_SOFTIRQ);
@@ -2031,7 +2028,6 @@
     raise_softirq_irqoff(NET_TX_SOFTIRQ);
 - Softirqs are most often raised from within interrupt handlers. In the case of interrupt handlers, the interrupt handler performs the basic hardware-related work, raises the softirq, and then exits.
 </t>
-    </r>
   </si>
   <si>
     <t>Tasklets</t>
@@ -2077,8 +2073,7 @@
     <t>Using Tasklets</t>
   </si>
   <si>
-    <r>
-      <t>
+    <t>
 - Declaring Your Tasklet
     - statically create the tasklet, use one of two macros in &lt;linux/interrupt.h&gt; :
         DECLARE_TASKLET(name, func, data)
@@ -2108,7 +2103,6 @@
         /* tasklet is now enabled */
 - You can remove a tasklet from the pending queue via tasklet_kill() .
 </t>
-    </r>
   </si>
   <si>
     <t>Work Queues</t>
@@ -3596,6 +3590,395 @@
     wait_queue_head_t poll; /* polling waitqueue */
     int event; /* event count */
 }; 
+</t>
+  </si>
+  <si>
+    <t>Block I/O Layer</t>
+  </si>
+  <si>
+    <t>Anatomy of a Block Device</t>
+  </si>
+  <si>
+    <t>
+- The smallest addressable unit on a block device is a sector. Sectors come in various powers of two, but 512 bytes is the most common size.
+- Software has different goals and therefore imposes its own smallest logically addressable unit, which is the block.
+- The block is an abstraction of the filesystem—filesystems can be accessed only in multiples of a block.Although the physical device is addressable at the sector level, the kernel performs all disk operations in terms of blocks.
+- Because the device’s smallest addressable unit is the sector, the block size can be no smaller than the sector and must be a multiple of a sector.
+- The kernel also requires that a block be no larger than the page size. Therefore, block sizes are a power-of-two multiple of the sector size and are not greater than the page size. Common block sizes are 512 bytes, 1 kilobyte, and 4 kilobytes.
+- Somewhat confusingly, some people refer to sectors and blocks with different names.
+    - Sectors, the smallest addressable unit to the device, are sometimes called “hard sectors” or “device blocks.” 
+    - Meanwhile, blocks, the smallest addressable unit to the filesystem, are sometimes referred to as “filesystem blocks” or “I/O blocks.”
+</t>
+  </si>
+  <si>
+    <t>Buffers and Buffer Heads</t>
+  </si>
+  <si>
+    <t>
+- When a block is stored in memory—say, after a read or pending a write—it is stored in a buffer. Each buffer is associated with exactly one block.
+- a single page can hold one or more blocks in memory. Because the kernel requires some associated control information to accompany the data (such as from which block device and which specific block the buffer is), each buffer is associated with a descriptor.The descriptor is called a buffer head and is of type struct buffer_head .
+- The buffer_head structure holds all the information that the kernel needs to manipulate buffers and is defined in &lt;linux/buffer_head.h&gt; .
+</t>
+  </si>
+  <si>
+    <t>
+- Take a look at this structure, with comments describing each field:
+    struct buffer_head {
+        unsigned long b_state; /* buffer state flags */
+        struct buffer_head *b_this_page; /* list of page’s buffers */
+        struct page *b_page; /* associated page */
+        sector_t b_blocknr; /* starting block number */
+        size_t b_size; /* size of mapping */
+        char *b_data; /* pointer to data within the page */
+        struct block_device *b_bdev; /* associated block device */
+        bh_end_io_t *b_end_io; /* I/O completion */
+        void *b_private; /* reserved for b_end_io */
+        struct list_head b_assoc_buffers; /* associated mappings */
+        struct address_space *b_assoc_map; /* associated address space */
+        atomic_t b_count; /* use count */
+    };
+</t>
+  </si>
+  <si>
+    <t>other are skipped</t>
+  </si>
+  <si>
+    <t>Devices and Modules</t>
+  </si>
+  <si>
+    <t>Device Types</t>
+  </si>
+  <si>
+    <t>
+- Block devices
+- Often abbreviated blkdevs, block devices are addressable in device-specified chunks called blocks and generally support seeking, the random access of data. 
+- Example block devices include hard drives, Blu-ray discs, and memory devices such as flash. 
+- Block devices are accessed via a special file called a block device node and generally mounted as a filesystem.
+- Character devices
+- Often abbreviated cdevs, character devices are generally not addressable, providing access to data only as a stream, generally of characters (bytes). 
+- Example character devices include keyboards, mice, printers, and most pseudo-devices. 
+- Character devices are accessed via a special file called a character device node. Unlike with block devices, applications interact with character devices directly through their device node.
+- Network devices
+- Sometimes called Ethernet devices after the most common type of network devices, network devices provide access to a network (such as the Internet) via a physical adapter (such as your laptop’s 802.11 card) and a specific protocol (such as IP). 
+- Breaking Unix’s “everything is a file” design principle, network devices are not accessed via a device node but with a special interface called the socket API.
+- Miscellaneous devices
+- Linux provides a handful of other device types, but they are specialized to a single task and not common.
+- One exception is miscellaneous devices, often abbreviated miscdevs, which are actually a simplified form of character devices. 
+- Miscellaneous devices enable a device driver author to represent simple devices easily, trading functionality for common infrastructure.
+- Pseudo devices
+- Not all device drivers represent physical devices. Some device drivers are virtual, providing access to kernel functionality.We call these pseudo devices; 
+- some of the most common are the kernel random number generator (accessible at /dev/random and /dev/urandom ), the null device (accessible at /dev/null ), the zero device (accessible at /dev/zero ), the full device (accessible at /dev/full ), and the memory device (accessible at /dev/mem ). Most device drivers, however, represent physical hardware.
+</t>
+  </si>
+  <si>
+    <t>Managing Configuration Options</t>
+  </si>
+  <si>
+    <t>
+- All you have to do is add an entry to the Kconfig file responsible for the applicable branch of the kernel source tree.
+    - For drivers, this is usually the directory in which the source lives. If the fishing pole driver lives in drivers/char/ , you use drivers/char/Kconfig.
+- If you created a new subdirectory and want a new Kconfig file to live there, you need to source it from an existing Kconfig.
+    - You do this by adding a line such as the following to an existing Kconfig file:
+    source “drivers/char/fishing/Kconfig”
+    - In this example, you would add this line to drivers/char/Kconfig. Entries in Kconfig are easy to add. Our fishing pole module would look like this:
+    config FISHING_POLE
+        tristate “Fish Master 3000 support”
+        default n
+        help
+        If you say Y here, support for the Fish Master 3000 with computer
+        interface will be compiled into the kernel and accessible via a
+        device node. You can also say M here and the driver will be built as a
+        module named fishing.ko.
+        If unsure, say N.    
+    - The first line defines what configuration option this entry represents. Note that the CONFIG_prefix is assumed and not written.
+    - The second line states that this option is a tristate, meaning that it can be built into the kernel (Y), built as a module (M), or not built at all (N).we can use the directive bool instead of tristate. The quoted text following the directive provides the name of this option in the various configuration utilities.
+    - The third line specifies the default for this option, which is not built ( n ).You can also specify the default as built into the kernel ( y ) or built as a module ( m ). For device drivers, the default is usually to not build it ( n ).
+    - The help directive signifies that the rest of the test, indented as it is, is the help text for this entry.
+</t>
+  </si>
+  <si>
+    <t>
+    - There are other options, too.The depends directive specifies options that must be set before this option can be set. If the dependencies are not met, the option is disabled.
+        - For example, if you added the following directive to the Kconfig entry, the device driver could not be enabled ( y or m ) until the CONFIG_FISH_TANK option is enabled:
+        depends on FISH_TANK
+    - The select directive is like depends , except that it forces the given option if our option is selected.The select directive should not be used as frequently as depends because it automatically enables other configuration options.
+        - The following line enables CONFIG_BAIT whenever CONFIG_FISHING_POLE is enabled:
+        select BAIT
+    - For both select and depends , you can request multiple options via &amp;&amp; .With depends , you can also specify that an option not be enabled by prefixing the option with an exclamation mark. 
+        - For example
+        depends on EXAMPLE_DRIVERS &amp;&amp; !NO_FISHING_ALLOWED
+        This line specifies that the driver depends on CONFIG_EXAMPLE_DRIVERS being set and CONFIG_NO_FISHING_ALLOWED being unset.
+    - The tristate and bool options can be followed by the directive if , which makes the entire option conditional on another configuration option. If the condition is not met, the configuration option is not only disabled but also does not appear in the configuration utilities. 
+        - For example, this directive instructs the configuration system to display an option only if CONFIG_OCEAN is set. Here, deep sea mode is available only if CONFIG_OCEAN is enabled:
+        bool “Deep Sea Mode” if OCEAN
+        The if directive can also follow the default directive, enforcing the default only if the conditional is met.
+    - The option CONFIG_DEBUG_KERNEL enables the selection of debugging-related options. Finally, the CONFIG_EXPERIMENTAL option is used to flag options that are experimental or otherwise of beta quality.
+</t>
+  </si>
+  <si>
+    <t>Module Parameters</t>
+  </si>
+  <si>
+    <t>
+- The macro does not declare the variable for you.You must do that before using the macro.Therefore, typical use might resemble.
+- module_param( name , type , perm );
+    - name is the name of both the parameter exposed to the user and the variable holding the parameter inside your module.
+    - The type argument holds the parameter’s data type; 
+    - it is one of byte , short , ushort , int , uint , long , ulong , charp , bool , or invbool. These types are, respectively, a byte, a short integer, an unsigned short integer, an integer, an unsigned integer, a long integer, an unsigned long integer, a pointer to a char , a Boolean, and a Boolean whose value is inverted from what the user specifies.The byte type is stored in a single char and the Boolean types are stored in variables of type int .
+    - The perm argument specifies the permissions of the corresponding file in sysfs.The permissions can be specified in the usual octal format, for example 0644 (owner can read and write, group can read, everyone else can read), or by ORing together the usual S_Ifoo defines.
+    - This would be in the outermost scope of your module’s source file. In other words, allow_live_bait is global to the file.
+- module_param_named( name , variable , type , perm );
+    - It is possible to have the internal variable named differently than the external parameter.This is accomplished via module_param_named() :
+    - Here, name is the externally viewable parameter name, and variable is the name of the internal global variable. For example
+- module_param_string( name , string , len , perm );
+    - it is also possible to have the kernel copy the string directly into a character array that you supply.This is done via module_param_string() :
+    - len is the size of the buffer named by string (or some smaller size, but that does not makemuch sense),
+    - perm is the sysfs permissions (or zero to disable a sysfs entry altogether).
+- module_param_array(name, type, nump, perm);
+- module_param_array_named( name , array , type , nump , perm );
+- MODULE_PARM_DESC(name, “Description”);  
+</t>
+  </si>
+  <si>
+    <t>
+    -   static int allow_live_bait = 1; /* default to on */
+        module_param(allow_live_bait, bool, 0644); /* a Boolean type */
+    -   static unsigned int max_test = DEFAULT_MAX_LINE_TEST;
+        module_param_named(maximum_line_test, max_test, int, 0);
+    -   static char species[BUF_LEN];
+        module_param_string(specifies, species, BUF_LEN, 0);
+    -   static int fish[MAX_FISH];
+        static int nr_fish;
+        module_param_array(fish, int, &amp;nr_fish, 0444);
+</t>
+  </si>
+  <si>
+    <t>Kobjects</t>
+  </si>
+  <si>
+    <t>
+- At the heart of the device model is the kobject, short for kernel object, which is represented by struct kobject and defined in &lt;linux/kobject.h&gt; .
+- It provides basic facilities, such as reference counting, a name, and a parent pointer, enabling the creation of a hierarchy of objects.
+- The sd pointer points to a sysfs_dirent structure that represents this kobject in sysfs. Inside this structure is an inode structure representing the kobject in the sysfs filesystem.
+- The kref structure provides reference counting.
+- The ktype and kset structures describe and group kobjects.
+- Kobjects are usually embedded in other structures and are generally not interesting on their own. Instead, a more important structure, such as struct cdev , defined in  &lt;linux/cdev.h&gt; , has a kobj member:
+- When kobjects are embedded inside other structures, the structures receive the stan dardized functions that a kobject provides. Most important, the structure’s embedded kobject now enables the structure to become part of an object hierarchy.
+</t>
+  </si>
+  <si>
+    <t>
+Struct kobject {
+    const char *name;
+    struct list_head entry;
+    struct kobject *parent;
+    struct kset *kset;
+    struct kobj_type *ktype;
+    struct sysfs_dirent *sd;
+    struct kref kref;
+    unsigned int state_initialized:1;
+    unsigned int state_in_sysfs:1;
+    unsigned int state_add_uevent_sent:1;
+    unsigned int state_remove_uevent_sent:1;
+    unsigned int uevent_suppress:1;
+};
+/* cdev structure - object representing a character device */
+struct cdev {
+    struct kobject kobj;
+    struct module *owner;
+    const struct file_operations *ops;
+    struct list_head list;
+    dev_t dev;
+    unsigned int count;
+};
+</t>
+  </si>
+  <si>
+    <t>ktype</t>
+  </si>
+  <si>
+    <r>
+      <t>
+- Kobjects are associated with a specific type, called a ktype.
+- Ktypes are represented by struct kobj_type and defined in &lt;linux/kobject.h&gt; :
+- Ktypes have the simple job of describing default behavior for a family of kobjects.
+- Instead of each kobject defining its own behavior, the behavior is stored in a ktype, and kobjects of the same “type” point at the same ktype structure, thus sharing the same behavior.
+- The release pointer points to the deconstructor called when a kobject’s reference count reaches zero.This function is responsible for freeing any memory associated with this kobject and otherwise cleaning up.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>
+Struct kobj_type {
+    void (*release)(struct kobject *);
+    const struct sysfs_ops *sysfs_ops;
+    struct attribute
+    **default_attrs;
+};
+</t>
+  </si>
+  <si>
+    <t>kset</t>
+  </si>
+  <si>
+    <t>
+- Ksets, short for kernel object sets, are aggregate collections of kobjects. Ksets work as the base container class for a set of kernel objects, collecting related kobjects, such as “all block devices,” together in a single place. 
+- Ksets might sound similar to ktypes and prompt the question,“Why have both?” Ksets group related kernel objects together, whereas ktypes enable kernel objects (functionally related or not) to share common operations.
+- The distinction is kept to allow kobjects of identical ktypes to be grouped into different ksets.That is, there are only a handful of ktypes, but many ksets, in the Linux kernel.
+- The kset pointer points at a kobject’s associated kset. ksets are represented by the kset structure, which is declared in &lt;linux/kobject.h&gt; :
+- In this structure, list is a linked list of all kobjects in this kset, list_lock is a spinlockprotecting this entry in the list, kobj is a kobject representing the base class for this set, and uevent_ops points to a structure that describes the hotplug behavior of kobjects in this kset.
+- Uevent, short for user events, is a mechanism for communicating with user-space information about the hotplugging and hot removal of devices from a system.
+</t>
+  </si>
+  <si>
+    <t>
+struct kset {
+    struct list_head list;
+    spinlock_t list_lock;
+    struct kobject kobj;
+    struct kset_uevent_ops *uevent_ops;
+};
+</t>
+  </si>
+  <si>
+    <t>Interrelation of Kobjects, Ktypes, and Ksets</t>
+  </si>
+  <si>
+    <t>
+- The important key object is the kobject, represented by struct kobject .The kobject introduces basic object properties—such as reference counting, parent-child relationship, and naming—to kernel data structures.The kobject structure provides these features in a standard unified way. Kobjects, in and of themselves, are not particularly useful. Instead, kobjects are typically embedded in other data structures, giving those containing structures the features of the kobject.
+- Kobjects are associated with a specific ktype, which is represented by struct kobj_type and pointed at by the ktype variable inside of the kobject. ktypes define some default properties of related kobjects: destruction behavior, sysfs behavior, and default attributes.The ktype structure is not well named; think of ktypes not as a grouping but as a set of shared operations.
+- Kobjects are then grouped into sets, called ksets, which are represented by struct kset . Ksets provide two functions. First, their embedded kobject acts as a base class for a group of kobjects. Second, ksets aggregate together related kobjects. In sysfs, kobjects are the individual directories in the filesystem. Related directories—say, perhaps all subdirectories of a given directory—might be in the same kset.
+</t>
+  </si>
+  <si>
+    <t>Managing and Manipulating Kobjects</t>
+  </si>
+  <si>
+    <r>
+      <t>
+- The first step in using a kobject is declaring and initializing it. this is done using following which is declared in &lt;linux/kobject.h&gt; :
+    struct kobject * kobject_create(void);
+- After initialization, the kobject’s reference count is set to one. So long as the reference count is nonzero, the object continues to exist in memory and is said to be pinned.
+    - When the code is finished with the object, the reference count is decremented. 
+    - When the reference count reaches zero, the object can be destroyed and any associated memory freed.
+    struct kobject * kobject_get(struct kobject *kobj); // increment reference count (getting)
+    void kobject_put(struct kobject *kobj); // decrement reference count (putting)
+</t>
+    </r>
+  </si>
+  <si>
+    <t>sysfs</t>
+  </si>
+  <si>
+    <t>
+- The magic behind sysfs is simply tying kobjects to directory entries via the dentry member inside each kobject.
+- The root of the sysfs contains at least 10 directories: block , bus , class , dev , devices , firmware , fs , kernel , module , and power .
+- The block directory contains one directory for each of the registered block devices on the system. Each of those directories, in turn, contains any partitions on the block device.
+- The bus directory provides a view of the system buses.
+- The class directory contains a view of the devices on the system organized by high-level function.
+- The dev directory is a view of registered device nodes.
+- The devices directory is a view of the device topology of the system. It maps directly to the hierarchy of device structures inside the kernel.
+- The firmware directory contains a system-specific tree of low-level subsystems such as ACPI, EDD, EFI, and so on.
+- The fs directory contains a view of registered filesystems.
+- The kernel directory contains kernel configuration options and status information.
+- the modules directory contains a view of the system’s loaded modules.
+- The power directory contains systemwide power management data.
+- Not all systems have all directories and yet other systems have directories not mentioned here.
+- The most important directory is devices , which exports the device model to the world.The directory structure is the actual device topology of the system. 
+- Much of the data in other directories is simply alternative organizations of the data in the devices directory. For example, /sys/class/net/ organizes devices by the high-level concept of registered network interfaces. Inside this directory might be the subdirectory eth0 , which contains the symlink device back to the actual device directory in devices .
+</t>
+  </si>
+  <si>
+    <t>Adding and Removing kobjects from sysfs</t>
+  </si>
+  <si>
+    <t>
+- Initialized kobjects are not automatically exported to sysfs.To represent a kobject to sysfs, you use kobject_add() :
+    int kobject_add(struct kobject *kobj, struct kobject *parent, const char *fmt, ...);
+- A given kobject’s location in sysfs depends on the kobject’s location in the object hierarchy. 
+- If the kobject’s parent pointer is set, the kobject maps to a subdirectory in sysfs inside its parent. 
+- If the parent pointer is not set, the kobject maps to a subdirectory inside kset-&gt;kobj.
+- If neither the parent nor the kset fields are set in the given kobject, the kobject is assumed to have no parent and maps to a root-level directory in sysfs. 
+- In most use cases, one or both of parent and kset should be set appropriately before kobject_add() is called.
+- Note that kobject_create_and_add() receives the name of the kobject’s directory as a direct pointer, name , while kobject_add() uses printf() -style formatting.
+- Removing a kobject’s sysfs representation is done via kobject_del() :
+    void kobject_del(struct kobject *kobj);
+- All of these functions are defined in lib/kobject.c and declared in &lt;linux/kobject.h&gt; .
+</t>
+  </si>
+  <si>
+    <t>
+- The helper function kobject_create_and_add() combines the work of kobject_create() and kobject_add() into one function:
+    struct kobject * kobject_create_and_add(const char *name, struct kobject *parent);
+</t>
+  </si>
+  <si>
+    <t>Adding Files to sysfs</t>
+  </si>
+  <si>
+    <t>
+- Default attributes
+- A default set of files is provided via the ktype field in kobjects and ksets. 
+- Consequently, all kobjects of the same type have the same default set of files populating their sysfs directories.
+- The kobj_type structure contains a member, default_attrs , that is an array of attribute structures. Attributes map kernel data to files in sysfs.
+- The name member provides the name of this attribute.This will be the filename of the resulting file in sysfs.
+- The owner member points to a module structure representing the owning module, if any. If a module does not own this attribute, this field is NULL .
+- The mode member is a mode_t type that specifies the permissions for the file in sysfs.
+- Although default_attrs lists the default attributes, sysfs_ops describes how to use them.
+- The show() method is invoked when the sysfs entry is read from user-space. It must copy the value of the attribute given by attr into the buffer provided by buffer .The buffer is PAGE_SIZE bytes in length; on x86, PAGE_SIZE is 4096 bytes.
+- The function should return the size in bytes of data actually written into buffer on success or a negative error code on failure.
+- The store() method is invoked on write. It must read the size bytes from buffer into the variable represented by the attribute attr .The size of the buffer is always PAGE_SIZE or smaller.
+- The function should return the size in bytes of data read from buffer on success or a negative error code on failure.
+- Creating New Attributes
+- some specific instance of a kobject is somehow special. It wants or even needs its own attributes—perhaps to provide data or functionality not shared by the more general ktype.To this end, the kernel provides the sysfs_create_file() interface
+- for adding new attributes on top of the default set:
+    int sysfs_create_file(struct kobject *kobj, const struct attribute *attr);
+- In addition to creating actual files, it is possible to create symbolic links. Creating a symlink in sysfs is easy:
+    int sysfs_create_link(struct kobject *kobj, struct kobject *target, char *name);    
+- Note that the sysfs_ops specified in the kobject’s ktype is invoked to handle this new attribute.The existing default show() and store() methods must be capable of handling the newly created attribute.
+- Destroying Attributes
+- Removing an attribute is handled via sysfs_remove_file() :
+    void sysfs_remove_file(struct kobject *kobj, const struct attribute *attr);
+- Upon call return, the given attribute no longer appears in the given kobject’s directory.
+- Symbolic links created with sysfs_create_link() can be removed with sysfs_remove_link() :
+    void sysfs_remove_link(struct kobject *kobj, char *name);
+</t>
+  </si>
+  <si>
+    <r>
+      <t>
+- default attributes
+    The attribute structure is defined in &lt;linux/sysfs.h&gt; :
+    /* attribute structure - attributes map kernel data to a sysfs file */
+    struct attribute {
+        const char *name; /* attribute’s name */
+        struct module *owner; /* owning module, if any */
+        mode_t mode; /* permissions */
+    };
+    - The sysfs_ops member is a pointer to a structure of the same name, which is defined in &lt;linux/sysfs.h&gt; :
+    struct sysfs_ops {
+        /* method invoked on read of a sysfs file */
+        ssize_t (*show) (struct kobject *kobj, struct attribute *attr, char *buffer);
+        /* method invoked on write of a sysfs file */
+        ssize_t (*store) (struct kobject *kobj, struct attribute *attr, const char *buffer, size_t size);
+    };
+</t>
+    </r>
+  </si>
+  <si>
+    <t>The Kernel Events Layer</t>
+  </si>
+  <si>
+    <t>
+- The Kernel Event Layer implements a kernel-to-user notification system on top of kobjects.
+- The Kernel Event Layer models events as signals emitting from objects—specifically, kobjects. Because kobjects map to sysfs paths, the source of each event is a sysfs path. If the event in question has to do with your first hard drive, /sys/block/hda is the source address. Internally, inside the kernel, we model the event as originating from the backing kobject.
+- Each event is given a verb or action string representing the signal.The strings are terms such as modified or unmounted that describe what happened. Finally, each event has an optional payload. Rather than pass an arbitrary string to user-space that provides the payload, the kernel event layer represents payloads as sysfs attributes.
+- Internally, the kernel events go from kernel-space out to user-space via netlink. Netlink is a high-speed multicast socket that transmits networking information. Using netlink means that obtaining kernel events from user-space is as simple as blocking on a socket.The intention is for user-space to implement a system daemon that listens on the socket, processes any read events, and transmits the events up the system stack.
+- To send events out to user-space from your kernel code, use kobject_uevent() :
+    int kobject_uevent(struct kobject *kobj, enum kobject_action action);
+    - The first parameter specifies the kobject emitting this signal.
+    - The second parameter specifies the action or verb describing this signal.The actual kernel event contains a string that maps to the provided enum kobject_action value.
+- This and related functions are defined in lib/kobject_uevent.c and declared in &lt;linux/kobject.h&gt; .
 </t>
   </si>
 </sst>
@@ -3708,7 +4091,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3731,6 +4114,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFEEEEEE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3333"/>
+        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
   </fills>
@@ -3775,7 +4164,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3936,6 +4325,14 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -3949,7 +4346,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFFF3333"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -6214,10 +6611,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F124"/>
+  <dimension ref="A1:F141"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E99" activeCellId="0" sqref="E99"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A141" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C141" activeCellId="0" sqref="C141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -7360,6 +7757,158 @@
       </c>
       <c r="E124" s="38" t="s">
         <v>593</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B125" s="38" t="s">
+        <v>594</v>
+      </c>
+      <c r="C125" s="38" t="s">
+        <v>595</v>
+      </c>
+      <c r="D125" s="38" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C126" s="38" t="s">
+        <v>597</v>
+      </c>
+      <c r="D126" s="38" t="s">
+        <v>598</v>
+      </c>
+      <c r="E126" s="38" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C127" s="40" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D128" s="37"/>
+    </row>
+    <row r="129" customFormat="false" ht="438.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B129" s="38" t="s">
+        <v>601</v>
+      </c>
+      <c r="C129" s="38" t="s">
+        <v>602</v>
+      </c>
+      <c r="D129" s="37" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="359.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C130" s="38" t="s">
+        <v>604</v>
+      </c>
+      <c r="D130" s="37" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="326.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D131" s="38" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="359.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C132" s="38" t="s">
+        <v>607</v>
+      </c>
+      <c r="D132" s="38" t="s">
+        <v>608</v>
+      </c>
+      <c r="E132" s="38" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="281.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C133" s="38" t="s">
+        <v>610</v>
+      </c>
+      <c r="D133" s="38" t="s">
+        <v>611</v>
+      </c>
+      <c r="E133" s="38" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C134" s="38" t="s">
+        <v>613</v>
+      </c>
+      <c r="D134" s="38" t="s">
+        <v>614</v>
+      </c>
+      <c r="E134" s="38" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C135" s="38" t="s">
+        <v>616</v>
+      </c>
+      <c r="D135" s="38" t="s">
+        <v>617</v>
+      </c>
+      <c r="E135" s="41" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C136" s="38" t="s">
+        <v>619</v>
+      </c>
+      <c r="D136" s="38" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C137" s="38" t="s">
+        <v>621</v>
+      </c>
+      <c r="D137" s="38" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="314.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C138" s="38" t="s">
+        <v>623</v>
+      </c>
+      <c r="D138" s="38" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C139" s="38" t="s">
+        <v>625</v>
+      </c>
+      <c r="D139" s="38" t="s">
+        <v>626</v>
+      </c>
+      <c r="E139" s="38" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="471.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C140" s="38" t="s">
+        <v>628</v>
+      </c>
+      <c r="D140" s="38" t="s">
+        <v>629</v>
+      </c>
+      <c r="E140" s="38" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="247.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C141" s="38" t="s">
+        <v>631</v>
+      </c>
+      <c r="D141" s="38" t="s">
+        <v>632</v>
       </c>
     </row>
   </sheetData>

</xml_diff>